<commit_message>
added logic for correctly mark attendance
</commit_message>
<xml_diff>
--- a/employee_attendance.xlsx
+++ b/employee_attendance.xlsx
@@ -16,9 +16,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="167" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -58,12 +60,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,12 +470,60 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>22:03:15</t>
+          <t>00:23:19</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" s="2" t="n">
-        <v>45632</v>
+        <v>45633</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Sunil</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>00:27:14</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" s="2" t="n">
+        <v>45633</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Sunil</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>00:28:37</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" s="2" t="n">
+        <v>45633</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Sunil</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>00:32:33</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" s="3" t="n">
+        <v>45633</v>
       </c>
     </row>
   </sheetData>

</xml_diff>